<commit_message>
Have cart show risky completions
</commit_message>
<xml_diff>
--- a/pub/chart.xlsx
+++ b/pub/chart.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>C</t>
   </si>
@@ -49,16 +49,16 @@
     <t>Ruby</t>
   </si>
   <si>
-    <t>Compile</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
     <t>Overall</t>
   </si>
   <si>
-    <t>Output</t>
+    <t>Successful compile</t>
+  </si>
+  <si>
+    <t>Successful run</t>
+  </si>
+  <si>
+    <t>Wrong output</t>
   </si>
 </sst>
 </file>
@@ -120,20 +120,20 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Output</c:v>
+                  <c:v>Wrong output</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>C</c:v>
                 </c:pt>
@@ -165,6 +165,39 @@
                   <c:v>Ruby</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Overall</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>C++</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C#</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Haskell</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Javascript</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Perl</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Overall</c:v>
                 </c:pt>
               </c:strCache>
@@ -172,42 +205,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9.6</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2</c:v>
+                  <c:v>18.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.6999999999999993</c:v>
+                  <c:v>22.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.4</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.1</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -222,16 +255,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Run</c:v>
+                  <c:v>Successful run</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>C</c:v>
                 </c:pt>
@@ -263,6 +296,39 @@
                   <c:v>Ruby</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Overall</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>C++</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C#</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Haskell</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Javascript</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Perl</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Overall</c:v>
                 </c:pt>
               </c:strCache>
@@ -316,20 +382,20 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Compile</c:v>
+                  <c:v>Successful compile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>C</c:v>
                 </c:pt>
@@ -361,6 +427,39 @@
                   <c:v>Ruby</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Overall</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>C++</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C#</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Haskell</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Java</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Javascript</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>PHP</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Perl</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Overall</c:v>
                 </c:pt>
               </c:strCache>
@@ -368,7 +467,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -411,11 +510,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="89332736"/>
-        <c:axId val="89380352"/>
+        <c:axId val="121601024"/>
+        <c:axId val="121606912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89332736"/>
+        <c:axId val="121601024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,14 +531,14 @@
             <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89380352"/>
+        <c:crossAx val="121606912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89380352"/>
+        <c:axId val="121606912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -457,7 +556,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                  <a:t>Success rate (%)</a:t>
+                  <a:t>Rate (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -477,7 +576,7 @@
             <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89332736"/>
+        <c:crossAx val="121601024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -494,13 +593,18 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.83951569556697869"/>
-          <c:y val="0.56898484289723117"/>
-          <c:w val="0.12906488116283496"/>
-          <c:h val="0.26911209937835662"/>
+          <c:x val="0.7505665839496577"/>
+          <c:y val="0.58850868005913326"/>
+          <c:w val="0.21183702771295415"/>
+          <c:h val="0.26911209937835667"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -846,23 +950,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -870,13 +979,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>9.6</v>
+        <v>29.3</v>
       </c>
       <c r="C2">
         <v>18.8</v>
       </c>
       <c r="D2">
-        <v>29.3</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -884,13 +993,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.5</v>
+        <v>19.8</v>
       </c>
       <c r="C3">
         <v>11.8</v>
       </c>
       <c r="D3">
-        <v>19.8</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -898,13 +1007,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.8</v>
+        <v>14.8</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>14.8</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -912,13 +1021,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.1</v>
+        <v>19.8</v>
       </c>
       <c r="C5">
         <v>17.899999999999999</v>
       </c>
       <c r="D5">
-        <v>19.8</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -926,13 +1035,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>17.3</v>
       </c>
       <c r="C6">
         <v>14.2</v>
       </c>
       <c r="D6">
-        <v>17.3</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -940,13 +1049,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5.2</v>
+        <v>49.9</v>
       </c>
       <c r="C7">
         <v>23.4</v>
       </c>
       <c r="D7">
-        <v>49.9</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -954,13 +1063,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>40.700000000000003</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>36.700000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -968,13 +1077,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>9.6999999999999993</v>
+        <v>43.9</v>
       </c>
       <c r="C9">
         <v>31.8</v>
       </c>
       <c r="D9">
-        <v>43.9</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -982,13 +1091,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>9.5</v>
+        <v>42.8</v>
       </c>
       <c r="C10">
         <v>24.3</v>
       </c>
       <c r="D10">
-        <v>42.8</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -996,27 +1105,192 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>15.4</v>
+        <v>52.1</v>
       </c>
       <c r="C11">
         <v>29.7</v>
       </c>
       <c r="D11">
-        <v>52.1</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>7.1</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="C12">
         <v>22.5</v>
       </c>
       <c r="D12">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>29.3</v>
+      </c>
+      <c r="C16">
+        <v>18.8</v>
+      </c>
+      <c r="D16">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>19.8</v>
+      </c>
+      <c r="C17">
+        <v>11.8</v>
+      </c>
+      <c r="D17">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>14.8</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>19.8</v>
+      </c>
+      <c r="C19">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D19">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>17.3</v>
+      </c>
+      <c r="C20">
+        <v>14.2</v>
+      </c>
+      <c r="D20">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>49.9</v>
+      </c>
+      <c r="C21">
+        <v>23.4</v>
+      </c>
+      <c r="D21">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="D22">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>43.9</v>
+      </c>
+      <c r="C23">
+        <v>31.8</v>
+      </c>
+      <c r="D23">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>42.8</v>
+      </c>
+      <c r="C24">
+        <v>24.3</v>
+      </c>
+      <c r="D24">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>52.1</v>
+      </c>
+      <c r="C25">
+        <v>29.7</v>
+      </c>
+      <c r="D25">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
         <v>33.700000000000003</v>
+      </c>
+      <c r="C26">
+        <v>22.5</v>
+      </c>
+      <c r="D26">
+        <v>15.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>